<commit_message>
Added Firearm Purchase Prohibition Code.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Firearm_Purchase_Prohibition_Query_Results/artifacts/service_model/information_model/IEPD/documentation/FirearmPurchaseProhibitionQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Firearm_Purchase_Prohibition_Query_Results/artifacts/service_model/information_model/IEPD/documentation/FirearmPurchaseProhibitionQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2720" windowWidth="30080" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="3460" yWindow="2040" windowWidth="30080" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Query Request Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>CLASS</t>
   </si>
@@ -98,6 +98,27 @@
   </si>
   <si>
     <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>Extension (code)</t>
+  </si>
+  <si>
+    <t>Firearm Purchase Prohibition Code</t>
+  </si>
+  <si>
+    <r>
+      <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/j:CourtOrder[@structures:id=../j:ActivityCourtOrderAssociation/j:CourtOrder/@structures:ref]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/me-fpp-codes:FirearmPurchaseProhibitionCode</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -197,9 +218,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="596">
+  <cellStyleXfs count="598">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -798,12 +821,6 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -824,8 +841,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="596">
+  <cellStyles count="598">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1123,6 +1146,7 @@
     <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1420,6 +1444,7 @@
     <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1750,143 +1775,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="97.1640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" s="2" customFormat="1">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="60">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="60">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="56" customHeight="1">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="56" customHeight="1">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="56" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="45">
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1"/>
-    <row r="16" spans="1:4" s="4" customFormat="1"/>
+    <row r="16" spans="1:4" s="2" customFormat="1"/>
+    <row r="17" s="2" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Added FirearmPurchaseProhibitionReason abstract element.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Firearm_Purchase_Prohibition_Query_Results/artifacts/service_model/information_model/IEPD/documentation/FirearmPurchaseProhibitionQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Firearm_Purchase_Prohibition_Query_Results/artifacts/service_model/information_model/IEPD/documentation/FirearmPurchaseProhibitionQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="2040" windowWidth="30080" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="4640" yWindow="1120" windowWidth="30080" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Query Request Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>CLASS</t>
   </si>
@@ -45,34 +45,9 @@
     <t>FIREARM PURCHASE PROHIBITION QUERY RESULTS IEPD</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Court Order</t>
-  </si>
-  <si>
     <t>Subject/Person</t>
   </si>
   <si>
-    <t>Docket ID</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Case[@structures:id=../j:ActivityCourtOrderAssociation/nc:Activity/@structures:ref]/nc:CaseDocketID</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/j:CourtOrder[@structures:id=../j:ActivityCourtOrderAssociation/j:CourtOrder/@structures:ref]
-/j:CourtOrderIssuingCourt/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>Court ORI</t>
-  </si>
-  <si>
-    <t>Court Order Issuing Date</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/j:CourtOrder[@structures:id=../j:ActivityCourtOrderAssociation/j:CourtOrder/@structures:ref]/j:CourtOrderIssuingDate/nc:Date</t>
-  </si>
-  <si>
     <t>DOB</t>
   </si>
   <si>
@@ -82,43 +57,34 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
-  </si>
-  <si>
-    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../j:ActivityCourtOrderAssociation/j:Subject/@structures:ref]/j:PersonSexCode</t>
-  </si>
-  <si>
     <t>Extension (code)</t>
   </si>
   <si>
     <t>Firearm Purchase Prohibition Code</t>
   </si>
   <si>
-    <r>
-      <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/j:CourtOrder[@structures:id=../j:ActivityCourtOrderAssociation/j:CourtOrder/@structures:ref]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/me-fpp-codes:FirearmPurchaseProhibitionCode</t>
-    </r>
+    <t>Firearm Purchase Prohibition</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../nc:ActivityPersonAssociation/nc:Person/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../nc:ActivityPersonAssociation/nc:Person/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../nc:ActivityPersonAssociation/nc:Person/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../nc:ActivityPersonAssociation/nc:Person/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../nc:ActivityPersonAssociation/nc:Person/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/nc:Person[@structures:id=../nc:ActivityPersonAssociation/nc:Person/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/fppq-res-doc:FirearmPurchaseProhibitionQueryResults/fppq-res-ext:FirearmPurchaseProhibitionReport/fppq-res-ext:FirearmPurchaseProhibition[@structures:id=../nc:ActivityPersonAssociation/nc:Activity/@structures:ref]/me-fpp-codes:FirearmPurchaseProhibitionCode</t>
   </si>
 </sst>
 </file>
@@ -218,9 +184,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="598">
+  <cellStyleXfs count="602">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -835,10 +805,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,7 +818,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="598">
+  <cellStyles count="602">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1147,6 +1117,8 @@
     <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1445,6 +1417,8 @@
     <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1775,16 +1749,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="97.1640625" style="1" customWidth="1"/>
@@ -1813,116 +1787,83 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
+    <row r="3" spans="1:4" s="6" customFormat="1">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="45">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    <row r="4" spans="1:4" s="6" customFormat="1" ht="45">
+      <c r="A4" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="60">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="45">
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="56" customHeight="1">
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="45">
       <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="56" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="45">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" ht="45">
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" ht="45">
       <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="45">
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="45">
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" ht="45">
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="45">
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1"/>
-    <row r="17" s="2" customFormat="1"/>
+    <row r="12" spans="1:4" s="2" customFormat="1"/>
+    <row r="13" spans="1:4" s="2" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>